<commit_message>
le excel des fonction
</commit_message>
<xml_diff>
--- a/Excel_Exercice01_MiseEnFormeEtGraphique_Charles-Edward_Gibeau.xlsx
+++ b/Excel_Exercice01_MiseEnFormeEtGraphique_Charles-Edward_Gibeau.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\cvm\court\soutien\remise-de-devoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B10AA0F-7F63-492B-946A-3048CEF2FE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0B568F-AD98-4687-8BFB-751EC79709C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B0EEB6E9-258A-4F43-A51A-2CA2E841E5F9}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{14A0A342-E161-493D-989D-C170CFD172CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0EEB6E9-258A-4F43-A51A-2CA2E841E5F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{14A0A342-E161-493D-989D-C170CFD172CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultat attendu" sheetId="1" r:id="rId1"/>
@@ -2741,6 +2741,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2794,7 +2808,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -3414,7 +3428,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -6925,7 +6939,7 @@
   <dimension ref="B1:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="1">
       <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
@@ -7400,12 +7414,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003344BE67D7EB984A84C06E190413FBFD" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47f970db01455029df431765be63e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9de94308-2297-4d04-a77d-26fce9df9395" xmlns:ns4="22375818-dcd7-42e4-9660-6b33e030de66" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="36af26dbc36b6288b7ddae45b32d7e9e" ns3:_="" ns4:_="">
     <xsd:import namespace="9de94308-2297-4d04-a77d-26fce9df9395"/>
@@ -7576,6 +7584,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0F10B16-3BA5-4DBB-9D9C-E801AA84B972}">
   <ds:schemaRefs>
@@ -7585,23 +7599,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37E9EC6D-36DB-4E19-8CE7-24B6CEB78323}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="22375818-dcd7-42e4-9660-6b33e030de66"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="9de94308-2297-4d04-a77d-26fce9df9395"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AF5AED0-9EFA-4824-BC63-124563E12A31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7618,4 +7615,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37E9EC6D-36DB-4E19-8CE7-24B6CEB78323}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="22375818-dcd7-42e4-9660-6b33e030de66"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="9de94308-2297-4d04-a77d-26fce9df9395"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>